<commit_message>
update the revenue file
</commit_message>
<xml_diff>
--- a/assets/revenue.xlsx
+++ b/assets/revenue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haifam/Downloads/businessgo/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\business_go\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C53326-DF2E-0343-A2F2-1296FF4A0BC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF888C35-EC11-47D3-B91A-FDCC3F88D33E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{1B4FE869-DBC9-C249-A397-2CC55566A06E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B4FE869-DBC9-C249-A397-2CC55566A06E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -866,11 +866,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF0C5FD-6067-6349-8616-139AC73CEB90}">
   <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
@@ -879,7 +879,7 @@
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -907,7 +907,7 @@
         <v>8481</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -921,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -935,7 +935,7 @@
         <v>9992</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -949,7 +949,7 @@
         <v>21419</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -963,7 +963,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -977,7 +977,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -991,7 +991,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>2895</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>21419</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>6441</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>3186</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>150</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>9112</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>6177</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>14734</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>14507</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>147</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>2762</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>6527</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>8946</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>2323</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>4082</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>3115</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>149</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>3729</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>15434</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>6616</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>3026</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>7506</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>5950</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>4220</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>61</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>6485</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>62</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>6276</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>65</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>3818</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>69</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>8204</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>5629</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>73</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>75</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>7255</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>5668</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>78</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>83</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>84</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>3059</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>151</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>4028</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>6543</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>3875</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>91</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>92</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>93</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>148</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>94</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>95</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>96</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>3448</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>97</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>2341</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>98</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>99</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>147</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>100</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>101</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>7565</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>102</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>103</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>146</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>5307</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>105</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>7217</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>106</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>10468</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>107</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>108</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>109</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>5349</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>110</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>12214</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>111</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>2789</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>112</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>8596</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>113</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>19739</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>114</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>8069</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>115</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>116</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>117</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>6818</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>119</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>120</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>121</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>148</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>122</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>3589</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>123</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>124</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>125</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>4807</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>126</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>127</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>4245</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>128</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>129</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>130</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>131</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>132</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>133</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>3383</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>134</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>7128</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>135</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>5247</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>136</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1828</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>137</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>13805</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>138</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>13836</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>139</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>5442</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>140</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>13771</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>141</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>142</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>1726</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>143</v>
       </c>

</xml_diff>